<commit_message>
small 180 data benchmark
</commit_message>
<xml_diff>
--- a/benchmark_stats.xlsx
+++ b/benchmark_stats.xlsx
@@ -408,70 +408,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="ti"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="ti"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="ti"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -590,17 +526,28 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="ti"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color indexed="64"/>
         </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -617,6 +564,59 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="ti"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="ti"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -861,11 +861,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-598632864"/>
-        <c:axId val="-598632320"/>
+        <c:axId val="1975485600"/>
+        <c:axId val="1975490496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-598632864"/>
+        <c:axId val="1975485600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -921,12 +921,12 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-598632320"/>
+        <c:crossAx val="1975490496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-598632320"/>
+        <c:axId val="1975490496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -983,7 +983,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-598632864"/>
+        <c:crossAx val="1975485600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1656,14 +1656,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E16" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E16" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="A1:E16"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="image sample(s)" dataDxfId="0" dataCellStyle="Note"/>
-    <tableColumn id="2" name="IoU threshold" dataDxfId="6"/>
-    <tableColumn id="3" name="Process Name" dataDxfId="5"/>
-    <tableColumn id="4" name="mAP" dataDxfId="4"/>
-    <tableColumn id="5" name="Avg. frame processing time" dataDxfId="3"/>
+    <tableColumn id="1" name="image sample(s)" dataDxfId="4" dataCellStyle="Note"/>
+    <tableColumn id="2" name="IoU threshold" dataDxfId="3"/>
+    <tableColumn id="3" name="Process Name" dataDxfId="2"/>
+    <tableColumn id="4" name="mAP" dataDxfId="1"/>
+    <tableColumn id="5" name="Avg. frame processing time" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1959,13 +1959,14 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
     <col min="1" max="1" width="18.19921875" customWidth="1"/>
     <col min="2" max="3" width="13.3984375" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="25.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2081,8 +2082,12 @@
       <c r="C7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
+      <c r="D7" s="10">
+        <v>5.9259259259259199E-2</v>
+      </c>
+      <c r="E7" s="11">
+        <v>3.6961416403452498E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="12">
@@ -2094,8 +2099,12 @@
       <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="13"/>
+      <c r="D8" s="1">
+        <v>0.50490740740740703</v>
+      </c>
+      <c r="E8" s="13">
+        <v>4.1585841443803499E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="12">
@@ -2107,8 +2116,12 @@
       <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="13"/>
+      <c r="D9" s="1">
+        <v>0.47638888888888797</v>
+      </c>
+      <c r="E9" s="13">
+        <v>1.22331076198154</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="12">
@@ -2120,8 +2133,12 @@
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="13"/>
+      <c r="D10" s="1">
+        <v>3.79629629629629E-2</v>
+      </c>
+      <c r="E10" s="13">
+        <v>9.5702332920498304E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="18" thickBot="1">
       <c r="A11" s="14">
@@ -2133,8 +2150,12 @@
       <c r="C11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
+      <c r="D11" s="16">
+        <v>6.4814814814814797E-2</v>
+      </c>
+      <c r="E11" s="17">
+        <v>13.6222740888595</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="8">
@@ -2146,8 +2167,12 @@
       <c r="C12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
+      <c r="D12" s="10">
+        <v>0</v>
+      </c>
+      <c r="E12" s="11">
+        <v>3.6544668674468997E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="12">
@@ -2159,8 +2184,12 @@
       <c r="C13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="13"/>
+      <c r="D13" s="1">
+        <v>5.5555555555555497E-3</v>
+      </c>
+      <c r="E13" s="13">
+        <v>4.1201056374443899E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="12">
@@ -2172,8 +2201,12 @@
       <c r="C14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="13"/>
+      <c r="D14" s="1">
+        <v>5.5555555555555497E-3</v>
+      </c>
+      <c r="E14" s="13">
+        <v>1.21208487749099</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="12">
@@ -2185,8 +2218,12 @@
       <c r="C15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="13"/>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="13">
+        <v>9.6208782990773498E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="18" thickBot="1">
       <c r="A16" s="14">
@@ -2198,8 +2235,12 @@
       <c r="C16" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="17"/>
+      <c r="D16" s="16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="17">
+        <v>13.6158024642202</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>